<commit_message>
korrektur kapitel_5 von steffen
</commit_message>
<xml_diff>
--- a/content/Anhang/Topologiebewertung_V4.xlsx
+++ b/content/Anhang/Topologiebewertung_V4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C81E61C-E431-4624-AA1A-93EDFA142FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABE24B5-CE77-455B-B5D3-83036D9FA5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bewertung" sheetId="1" r:id="rId1"/>
@@ -1191,25 +1191,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F37"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="39" t="s">
         <v>49</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="34" t="s">
         <v>45</v>
       </c>
@@ -1259,22 +1259,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="35"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="48">
-        <f>3*4.8</f>
-        <v>14.399999999999999</v>
+        <f>17.64</f>
+        <v>17.64</v>
       </c>
       <c r="D3" s="48">
         <f>3*0.5*(D2*10^-6)*(260)^2</f>
         <v>1.7744999999999997</v>
       </c>
       <c r="E3" s="48">
-        <f>3*0.5*(E2*10^-6)*(260)^2</f>
-        <v>0.1014</v>
+        <v>0.13</v>
       </c>
       <c r="F3" s="48">
         <f t="shared" ref="F3" si="0">3*0.5*(F2*10^-6)*(260)^2</f>
@@ -1285,7 +1284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="35"/>
       <c r="B4" s="1" t="s">
         <v>42</v>
@@ -1307,7 +1306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="35"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -1333,7 +1332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="35"/>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1359,7 +1358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="35"/>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -1381,7 +1380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="35"/>
       <c r="B8" s="1" t="s">
         <v>44</v>
@@ -1393,8 +1392,8 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="E8" s="48">
-        <v>2.6461999999999999</v>
+      <c r="E8">
+        <v>8.82</v>
       </c>
       <c r="F8" s="48">
         <v>0</v>
@@ -1402,14 +1401,14 @@
       <c r="G8" s="11"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="35"/>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="12">
         <f>(C3+C6+C8)</f>
-        <v>22.214627999999998</v>
+        <v>25.454628</v>
       </c>
       <c r="D9" s="12">
         <f>(D3+D6+D8)</f>
@@ -1417,7 +1416,7 @@
       </c>
       <c r="E9" s="12">
         <f>(E3+E6+E8)</f>
-        <v>10.562227999999999</v>
+        <v>16.764628000000002</v>
       </c>
       <c r="F9" s="12">
         <f>(F3+F6+F8)</f>
@@ -1426,7 +1425,7 @@
       <c r="G9" s="24"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="36"/>
       <c r="B10" s="25" t="s">
         <v>39</v>
@@ -1437,22 +1436,22 @@
       </c>
       <c r="D10" s="43">
         <f t="shared" ref="D10:F10" si="3">(D9)/(MAX($C$9:$F$9))</f>
-        <v>0.43165827489886394</v>
+        <v>0.37671452122576682</v>
       </c>
       <c r="E10" s="43">
         <f t="shared" si="3"/>
-        <v>0.47546274463835275</v>
+        <v>0.6586082499418181</v>
       </c>
       <c r="F10" s="43">
         <f t="shared" si="3"/>
-        <v>0.43165827489886394</v>
+        <v>0.37671452122576682</v>
       </c>
       <c r="G10" s="37">
         <v>0.5</v>
       </c>
       <c r="H10" s="30"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="42" t="s">
         <v>46</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="35"/>
       <c r="B12" s="1" t="s">
         <v>43</v>
@@ -1498,7 +1497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="35"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1520,7 +1519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" s="35"/>
       <c r="B14" s="3" t="s">
         <v>12</v>
@@ -1544,7 +1543,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="36"/>
       <c r="B15" s="25" t="s">
         <v>38</v>
@@ -1570,7 +1569,7 @@
       </c>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="38" t="s">
         <v>17</v>
       </c>
@@ -1592,7 +1591,7 @@
       <c r="G16" s="33"/>
       <c r="H16" s="28"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="23"/>
       <c r="B17" s="1" t="s">
         <v>19</v>
@@ -1612,7 +1611,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="23"/>
       <c r="B18" s="1" t="s">
         <v>20</v>
@@ -1632,7 +1631,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23"/>
       <c r="B19" s="3" t="s">
         <v>12</v>
@@ -1656,7 +1655,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
         <v>37</v>
@@ -1682,7 +1681,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
       <c r="B21" s="50" t="s">
         <v>21</v>
@@ -1702,7 +1701,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="51"/>
       <c r="B22" s="52" t="s">
         <v>35</v>
@@ -1728,7 +1727,7 @@
       </c>
       <c r="H22" s="51"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="31" t="s">
         <v>22</v>
       </c>
@@ -1745,12 +1744,12 @@
         <v>7</v>
       </c>
       <c r="F23" s="32">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G23" s="33"/>
       <c r="H23" s="28"/>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4"/>
       <c r="B24" s="3" t="s">
         <v>12</v>
@@ -1769,37 +1768,37 @@
       </c>
       <c r="F24" s="12">
         <f>F23</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="6"/>
       <c r="B25" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="44">
         <f>(C24)/(MAX($C$23:$F$23))</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="D25" s="44">
         <f t="shared" ref="D25:F25" si="7">(D24)/(MAX($C$23:$F$23))</f>
-        <v>0.58333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="E25" s="44">
         <f t="shared" si="7"/>
-        <v>0.58333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="F25" s="44">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G25" s="13">
         <v>0.05</v>
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="18" t="s">
         <v>47</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -1849,7 +1848,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -1873,7 +1872,7 @@
       <c r="G28" s="15"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="23"/>
       <c r="B29" s="3" t="s">
         <v>27</v>
@@ -1896,7 +1895,7 @@
       <c r="G29" s="15"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
         <v>28</v>
@@ -1922,7 +1921,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="23"/>
       <c r="B31" s="1" t="s">
         <v>29</v>
@@ -1944,7 +1943,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="23"/>
       <c r="B32" s="1" t="s">
         <v>30</v>
@@ -1968,7 +1967,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="23"/>
       <c r="B33" s="3" t="s">
         <v>31</v>
@@ -1992,7 +1991,7 @@
       <c r="G33" s="15"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="23"/>
       <c r="B34" s="1" t="s">
         <v>32</v>
@@ -2016,7 +2015,7 @@
       <c r="G34" s="15"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="23"/>
       <c r="B35" s="3" t="s">
         <v>12</v>
@@ -2040,7 +2039,7 @@
       <c r="G35" s="24"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" s="62" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="62" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="57"/>
       <c r="B36" s="58" t="s">
         <v>40</v>
@@ -2066,7 +2065,7 @@
       </c>
       <c r="H36" s="61"/>
     </row>
-    <row r="37" spans="1:8" s="9" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="9" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A37" s="31" t="s">
         <v>33</v>
       </c>
@@ -2075,19 +2074,19 @@
       </c>
       <c r="C37" s="56">
         <f>C10*$G$10+C15*$G$15+C20*$G$20+C25*$G$25+C36*$G$36+C22*$G$22</f>
-        <v>0.77098077327505921</v>
+        <v>0.78764743994172592</v>
       </c>
       <c r="D37" s="56">
         <f>D10*$G$10+D15*$G$15+D20*$G$20+D25*$G$25+D36*$G$36+D22*$G$22</f>
-        <v>0.60042986819106314</v>
+        <v>0.58754132468784792</v>
       </c>
       <c r="E37" s="56">
         <f>E10*$G$10+E15*$G$15+E20*$G$20+E25*$G$25+E36*$G$36+E22*$G$22</f>
-        <v>0.64689803898584319</v>
+        <v>0.75305412497090907</v>
       </c>
       <c r="F37" s="56">
         <f>F10*$G$10+F15*$G$15+F20*$G$20+F25*$G$25+F36*$G$36+F22*$G$22</f>
-        <v>0.55028424315997315</v>
+        <v>0.51031236632342458</v>
       </c>
       <c r="G37" s="27">
         <f>SUM(G2:G36)</f>
@@ -2095,24 +2094,24 @@
       </c>
       <c r="H37" s="55"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="6"/>
       <c r="B38" s="49"/>
       <c r="C38" s="8">
         <f>(1-C37)*100</f>
-        <v>22.901922672494081</v>
+        <v>21.235256005827409</v>
       </c>
       <c r="D38" s="8">
         <f>(1-D37)*100</f>
-        <v>39.957013180893682</v>
+        <v>41.245867531215211</v>
       </c>
       <c r="E38" s="8">
         <f>(1-E37)*100</f>
-        <v>35.310196101415684</v>
+        <v>24.694587502909094</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" ref="F38" si="11">(1-F37)*100</f>
-        <v>44.971575684002687</v>
+        <v>48.968763367657544</v>
       </c>
       <c r="G38" s="49" t="s">
         <v>36</v>

</xml_diff>